<commit_message>
adding comment headers to all py files
</commit_message>
<xml_diff>
--- a/config_p3388/tv_generation_catalog.xlsx
+++ b/config_p3388/tv_generation_catalog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\meas\p3388_general_rfi_tv\config_p3388\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\meas\p3388_rfigen_ai.py\config_p3388\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B35297E-9452-49BB-AE54-3671A26461A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7461C262-1F76-4A70-BB05-69BDC4141734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="1875" windowWidth="17085" windowHeight="15915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,7 +439,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +484,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -498,7 +498,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -512,7 +512,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -526,7 +526,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -540,7 +540,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -554,7 +554,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -568,7 +568,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -582,7 +582,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -596,7 +596,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
@@ -610,7 +610,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
@@ -624,7 +624,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>

</xml_diff>